<commit_message>
v1.1 Update some test cases after first Review
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_REGISTERATION.xlsx
+++ b/LH_TESTCASES/LH_TC_REGISTERATION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEE8FD9-4758-49A4-9B61-309942C63213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A1BF42-3F08-4D80-A0CC-9864DE102138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F93099EE-3EF1-457C-A7E2-767E46A5A638}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F93099EE-3EF1-457C-A7E2-767E46A5A638}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_REGISTERATION" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
   <si>
     <t>Project name</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>Error message: "Password must be at least 8 characters long." (displayed next to the password field).</t>
-  </si>
-  <si>
-    <t>Verify error for password missing number/special character.</t>
   </si>
   <si>
     <t>Error message: "Password must include at least 1 number, 1 letter, and 1 special character."</t>
@@ -311,31 +308,43 @@
 SRS-REG-009.1</t>
   </si>
   <si>
-    <t>1. Enter valid email.
-2. Enter valid username.
-3. Enter valid password.
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Updated section</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Initial creation of Registration Test Cases</t>
+  </si>
+  <si>
+    <t>Omar Sherif</t>
+  </si>
+  <si>
+    <t>1. Enter an email in the format name@domain.com
+2. Enter valid username.(6–20 characters, letters/numbers/underscores only)
+3. Enter a password with at least 8 characters, including uppercase, lowercase, digit, and special character
 4. Click Register.</t>
   </si>
   <si>
-    <t>Version number</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Updated section</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>v1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Initial creation of Registration Test Cases</t>
-  </si>
-  <si>
-    <t>Omar Sherif</t>
+    <t>Verify error for password missing special character.</t>
+  </si>
+  <si>
+    <t>Verify error for password missing number.</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update some test cases after first Review </t>
   </si>
 </sst>
 </file>
@@ -345,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,14 +421,6 @@
       <b/>
       <i/>
       <sz val="14"/>
-      <color rgb="FF404040"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -442,6 +443,22 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -604,49 +621,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="12" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,9 +664,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -668,29 +673,41 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="13" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="13" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1035,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1991551B-C569-4A7F-A980-7316BEA92180}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="56" workbookViewId="0">
-      <selection activeCell="AL23" sqref="AL23"/>
+    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -1056,48 +1073,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="1"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
@@ -1141,311 +1158,311 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="28" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:10" s="16" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="E9" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19" t="s">
+      <c r="H9" s="33"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="27" customFormat="1" ht="54" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:10" s="15" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+      <c r="A10" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="38"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.4">
+      <c r="A11" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.4">
+      <c r="A12" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="43"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.4">
+      <c r="A13" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="B13" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25" t="s">
+      <c r="E13" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="14" customFormat="1" ht="54" x14ac:dyDescent="0.4">
-      <c r="A11" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="17" t="s">
+    <row r="14" spans="1:10" s="7" customFormat="1" ht="54" x14ac:dyDescent="0.4">
+      <c r="A14" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19" t="s">
+      <c r="E14" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="38"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.4">
-      <c r="A12" s="20" t="s">
+    <row r="15" spans="1:10" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.4">
+      <c r="A15" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="44"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.4">
+      <c r="A16" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="38"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.4">
+      <c r="A17" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="44"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="7" customFormat="1" ht="54" x14ac:dyDescent="0.4">
+      <c r="A18" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="38"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.4">
+      <c r="A19" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="22" t="s">
+      <c r="B19" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.4">
-      <c r="A13" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="7" customFormat="1" ht="54" x14ac:dyDescent="0.4">
-      <c r="A14" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.4">
-      <c r="A15" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.4">
-      <c r="A16" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.4">
-      <c r="A17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" ht="54" x14ac:dyDescent="0.4">
-      <c r="A18" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="20"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.4">
-      <c r="A19" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="26" t="s">
+      <c r="E19" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="F19" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19" t="s">
+      <c r="H19" s="44"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1538,66 +1555,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2880C1-311C-4561-94F0-88FDBC886A75}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="57" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.77734375" style="44" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" style="44" customWidth="1"/>
-    <col min="3" max="3" width="38" style="44" customWidth="1"/>
-    <col min="4" max="4" width="62.21875" style="44" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="44"/>
+    <col min="1" max="1" width="47.77734375" style="26" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="38" style="26" customWidth="1"/>
+    <col min="4" max="4" width="62.21875" style="26" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="D1" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="38" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="B2" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="D2" s="23">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="41">
-        <v>45766</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="41"/>
+      <c r="C3" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="23">
+        <v>45768</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="43"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="25"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v2.1 Executing Test Cases
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_REGISTERATION.xlsx
+++ b/LH_TESTCASES/LH_TC_REGISTERATION.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_TESTCASES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\LH_TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1A5C9E-311B-4AE9-AAD5-A4D985DB68E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F93099EE-3EF1-457C-A7E2-767E46A5A638}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_REGISTERATION" sheetId="1" r:id="rId1"/>
     <sheet name="Version History" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
   <si>
     <t>Project name</t>
   </si>
@@ -483,23 +482,61 @@
 Password: Pass@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">not excuted </t>
-  </si>
-  <si>
     <t>v2.0</t>
   </si>
   <si>
     <t>Update some test cases after Review of Ahmed</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>1. "Invalid Data" Message appears above the email field.</t>
+  </si>
+  <si>
+    <t>1. Account created succsessfully.
+2. user redirected to login page.
+3.Data stored in the database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password Rules Bubble section appears successfully </t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. "Invalid Data" Message appears for email and passward fields </t>
+  </si>
+  <si>
+    <t>1. "Invalid Data" Message appears under username field</t>
+  </si>
+  <si>
+    <t>1. "Invalid Data" Message appears under password field</t>
+  </si>
+  <si>
+    <t>1. "Invalid Data" Message appears under the email field.</t>
+  </si>
+  <si>
+    <t>1. "Invalid Data" Message appears under username field and all fields</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executing Test Cases </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -890,6 +927,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1258,38 +1298,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1991551B-C569-4A7F-A980-7316BEA92180}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FI66"/>
   <sheetViews>
-    <sheetView topLeftCell="B41" zoomScale="52" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="31" style="13" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="51.6640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="72.5546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="55.5546875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="21.109375" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="11"/>
+    <col min="2" max="2" width="48.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="72.5703125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="55.5703125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:165" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:165" s="9" customFormat="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="55"/>
       <c r="E1" s="41"/>
       <c r="F1" s="42"/>
       <c r="G1" s="42"/>
@@ -1420,15 +1460,15 @@
       <c r="EB1" s="42"/>
       <c r="EC1" s="42"/>
     </row>
-    <row r="2" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:165">
       <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="44"/>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
@@ -1559,15 +1599,15 @@
       <c r="EB2" s="37"/>
       <c r="EC2" s="37"/>
     </row>
-    <row r="3" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:165">
       <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="44"/>
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
@@ -1698,15 +1738,15 @@
       <c r="EB3" s="37"/>
       <c r="EC3" s="37"/>
     </row>
-    <row r="4" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:165">
       <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="44"/>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
@@ -1837,7 +1877,7 @@
       <c r="EB4" s="37"/>
       <c r="EC4" s="37"/>
     </row>
-    <row r="5" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:165">
       <c r="A5" s="46"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -1972,7 +2012,7 @@
       <c r="EB5" s="37"/>
       <c r="EC5" s="37"/>
     </row>
-    <row r="6" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:165">
       <c r="A6" s="46"/>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
@@ -2107,14 +2147,14 @@
       <c r="EB6" s="37"/>
       <c r="EC6" s="37"/>
     </row>
-    <row r="7" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:165">
       <c r="A7" s="46"/>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:165" s="35" customFormat="1" ht="73.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:165" s="35" customFormat="1" ht="36">
       <c r="A8" s="35" t="s">
         <v>5</v>
       </c>
@@ -2136,7 +2176,7 @@
       <c r="G8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="49" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="35" t="s">
@@ -2301,7 +2341,7 @@
       <c r="FH8" s="36"/>
       <c r="FI8" s="36"/>
     </row>
-    <row r="9" spans="1:165" s="28" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:165" s="28" customFormat="1" ht="229.5" customHeight="1">
       <c r="A9" s="30" t="s">
         <v>19</v>
       </c>
@@ -2323,9 +2363,11 @@
       <c r="G9" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="H9" s="33"/>
+      <c r="H9" s="33" t="s">
+        <v>131</v>
+      </c>
       <c r="I9" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J9" s="30" t="s">
         <v>15</v>
@@ -2486,7 +2528,7 @@
       <c r="FH9" s="20"/>
       <c r="FI9" s="20"/>
     </row>
-    <row r="10" spans="1:165" s="18" customFormat="1" ht="117" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:165" s="18" customFormat="1" ht="116.25">
       <c r="A10" s="21" t="s">
         <v>21</v>
       </c>
@@ -2508,16 +2550,18 @@
       <c r="G10" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="I10" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J10" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:165" s="29" customFormat="1" ht="117" x14ac:dyDescent="0.45">
-      <c r="A11" s="49" t="s">
+    <row r="11" spans="1:165" s="29" customFormat="1" ht="116.25">
+      <c r="A11" s="50" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="24" t="s">
@@ -2538,9 +2582,11 @@
       <c r="G11" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="27" t="s">
+        <v>136</v>
+      </c>
       <c r="I11" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>15</v>
@@ -2701,8 +2747,8 @@
       <c r="FH11" s="18"/>
       <c r="FI11" s="18"/>
     </row>
-    <row r="12" spans="1:165" s="29" customFormat="1" ht="70.2" x14ac:dyDescent="0.45">
-      <c r="A12" s="50"/>
+    <row r="12" spans="1:165" s="29" customFormat="1" ht="234.75" customHeight="1">
+      <c r="A12" s="51"/>
       <c r="B12" s="24" t="s">
         <v>54</v>
       </c>
@@ -2721,9 +2767,11 @@
       <c r="G12" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="33" t="s">
+        <v>131</v>
+      </c>
       <c r="I12" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J12" s="24" t="s">
         <v>15</v>
@@ -2884,8 +2932,8 @@
       <c r="FH12" s="18"/>
       <c r="FI12" s="18"/>
     </row>
-    <row r="13" spans="1:165" s="29" customFormat="1" ht="70.2" x14ac:dyDescent="0.45">
-      <c r="A13" s="51"/>
+    <row r="13" spans="1:165" s="29" customFormat="1" ht="238.5" customHeight="1">
+      <c r="A13" s="52"/>
       <c r="B13" s="24" t="s">
         <v>58</v>
       </c>
@@ -2904,9 +2952,11 @@
       <c r="G13" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="27" t="s">
+        <v>131</v>
+      </c>
       <c r="I13" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>15</v>
@@ -3067,7 +3117,7 @@
       <c r="FH13" s="18"/>
       <c r="FI13" s="18"/>
     </row>
-    <row r="14" spans="1:165" s="18" customFormat="1" ht="117" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:165" s="18" customFormat="1" ht="116.25">
       <c r="A14" s="17" t="s">
         <v>34</v>
       </c>
@@ -3089,15 +3139,17 @@
       <c r="G14" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="15"/>
+      <c r="H14" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="I14" s="48" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J14" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:165" s="29" customFormat="1" ht="117" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:165" s="29" customFormat="1" ht="116.25">
       <c r="A15" s="24" t="s">
         <v>23</v>
       </c>
@@ -3119,9 +3171,11 @@
       <c r="G15" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="27" t="s">
+        <v>136</v>
+      </c>
       <c r="I15" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J15" s="24" t="s">
         <v>67</v>
@@ -3282,7 +3336,7 @@
       <c r="FH15" s="18"/>
       <c r="FI15" s="18"/>
     </row>
-    <row r="16" spans="1:165" s="18" customFormat="1" ht="117" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:165" s="18" customFormat="1" ht="116.25">
       <c r="A16" s="17" t="s">
         <v>35</v>
       </c>
@@ -3304,15 +3358,17 @@
       <c r="G16" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="H16" s="15"/>
+      <c r="H16" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="I16" s="48" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J16" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:165" s="29" customFormat="1" ht="70.2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:165" s="29" customFormat="1" ht="69.75">
       <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
@@ -3334,9 +3390,11 @@
       <c r="G17" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="25"/>
+      <c r="H17" s="27" t="s">
+        <v>132</v>
+      </c>
       <c r="I17" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J17" s="24" t="s">
         <v>76</v>
@@ -3497,7 +3555,7 @@
       <c r="FH17" s="18"/>
       <c r="FI17" s="18"/>
     </row>
-    <row r="18" spans="1:165" s="18" customFormat="1" ht="70.2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:165" s="18" customFormat="1" ht="69.75">
       <c r="A18" s="17" t="s">
         <v>24</v>
       </c>
@@ -3519,15 +3577,17 @@
       <c r="G18" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="14"/>
+      <c r="H18" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="I18" s="48" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J18" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:165" s="29" customFormat="1" ht="117" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:165" s="29" customFormat="1" ht="116.25">
       <c r="A19" s="24" t="s">
         <v>37</v>
       </c>
@@ -3549,9 +3609,11 @@
       <c r="G19" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="27"/>
+      <c r="H19" s="27" t="s">
+        <v>130</v>
+      </c>
       <c r="I19" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J19" s="24" t="s">
         <v>15</v>
@@ -3712,7 +3774,7 @@
       <c r="FH19" s="18"/>
       <c r="FI19" s="18"/>
     </row>
-    <row r="20" spans="1:165" s="18" customFormat="1" ht="70.2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:165" s="18" customFormat="1" ht="69.75">
       <c r="A20" s="17" t="s">
         <v>38</v>
       </c>
@@ -3734,16 +3796,18 @@
       <c r="G20" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="15"/>
+      <c r="H20" s="14" t="s">
+        <v>134</v>
+      </c>
       <c r="I20" s="48" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J20" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:165" s="29" customFormat="1" ht="117" x14ac:dyDescent="0.45">
-      <c r="A21" s="49" t="s">
+    <row r="21" spans="1:165" s="29" customFormat="1" ht="116.25">
+      <c r="A21" s="50" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -3764,9 +3828,11 @@
       <c r="G21" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="24"/>
+      <c r="H21" s="27" t="s">
+        <v>135</v>
+      </c>
       <c r="I21" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J21" s="24" t="s">
         <v>15</v>
@@ -3927,8 +3993,8 @@
       <c r="FH21" s="18"/>
       <c r="FI21" s="18"/>
     </row>
-    <row r="22" spans="1:165" s="29" customFormat="1" ht="117" x14ac:dyDescent="0.45">
-      <c r="A22" s="50"/>
+    <row r="22" spans="1:165" s="29" customFormat="1" ht="201" customHeight="1">
+      <c r="A22" s="51"/>
       <c r="B22" s="24" t="s">
         <v>93</v>
       </c>
@@ -3947,9 +4013,11 @@
       <c r="G22" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="H22" s="24"/>
+      <c r="H22" s="27" t="s">
+        <v>131</v>
+      </c>
       <c r="I22" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J22" s="24" t="s">
         <v>15</v>
@@ -4110,8 +4178,8 @@
       <c r="FH22" s="18"/>
       <c r="FI22" s="18"/>
     </row>
-    <row r="23" spans="1:165" s="29" customFormat="1" ht="117" x14ac:dyDescent="0.45">
-      <c r="A23" s="50"/>
+    <row r="23" spans="1:165" s="29" customFormat="1" ht="216" customHeight="1">
+      <c r="A23" s="51"/>
       <c r="B23" s="24" t="s">
         <v>97</v>
       </c>
@@ -4130,9 +4198,11 @@
       <c r="G23" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="H23" s="24"/>
+      <c r="H23" s="27" t="s">
+        <v>131</v>
+      </c>
       <c r="I23" s="34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J23" s="24" t="s">
         <v>15</v>
@@ -4293,8 +4363,8 @@
       <c r="FH23" s="18"/>
       <c r="FI23" s="18"/>
     </row>
-    <row r="24" spans="1:165" s="29" customFormat="1" ht="117" x14ac:dyDescent="0.45">
-      <c r="A24" s="51"/>
+    <row r="24" spans="1:165" s="29" customFormat="1" ht="116.25">
+      <c r="A24" s="52"/>
       <c r="B24" s="24" t="s">
         <v>100</v>
       </c>
@@ -4313,9 +4383,11 @@
       <c r="G24" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="H24" s="24"/>
+      <c r="H24" s="27" t="s">
+        <v>135</v>
+      </c>
       <c r="I24" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J24" s="24" t="s">
         <v>15</v>
@@ -4476,7 +4548,7 @@
       <c r="FH24" s="18"/>
       <c r="FI24" s="18"/>
     </row>
-    <row r="25" spans="1:165" s="19" customFormat="1" ht="117" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:165" s="19" customFormat="1" ht="116.25">
       <c r="A25" s="17" t="s">
         <v>40</v>
       </c>
@@ -4498,15 +4570,17 @@
       <c r="G25" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="17"/>
+      <c r="H25" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="I25" s="48" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:165" s="29" customFormat="1" ht="70.2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:165" s="29" customFormat="1" ht="69.75">
       <c r="A26" s="24" t="s">
         <v>41</v>
       </c>
@@ -4528,9 +4602,11 @@
       <c r="G26" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="H26" s="24"/>
+      <c r="H26" s="27" t="s">
+        <v>138</v>
+      </c>
       <c r="I26" s="34" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J26" s="24" t="s">
         <v>67</v>
@@ -4691,7 +4767,7 @@
       <c r="FH26" s="18"/>
       <c r="FI26" s="18"/>
     </row>
-    <row r="27" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:165">
       <c r="K27" s="37"/>
       <c r="L27" s="37"/>
       <c r="M27" s="37"/>
@@ -4848,7 +4924,7 @@
       <c r="FH27" s="37"/>
       <c r="FI27" s="37"/>
     </row>
-    <row r="28" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:165">
       <c r="K28" s="37"/>
       <c r="L28" s="37"/>
       <c r="M28" s="37"/>
@@ -5005,7 +5081,7 @@
       <c r="FH28" s="37"/>
       <c r="FI28" s="37"/>
     </row>
-    <row r="29" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:165">
       <c r="K29" s="37"/>
       <c r="L29" s="37"/>
       <c r="M29" s="37"/>
@@ -5162,7 +5238,7 @@
       <c r="FH29" s="37"/>
       <c r="FI29" s="37"/>
     </row>
-    <row r="30" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:165">
       <c r="K30" s="37"/>
       <c r="L30" s="37"/>
       <c r="M30" s="37"/>
@@ -5319,7 +5395,7 @@
       <c r="FH30" s="37"/>
       <c r="FI30" s="37"/>
     </row>
-    <row r="31" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:165">
       <c r="K31" s="37"/>
       <c r="L31" s="37"/>
       <c r="M31" s="37"/>
@@ -5476,7 +5552,7 @@
       <c r="FH31" s="37"/>
       <c r="FI31" s="37"/>
     </row>
-    <row r="32" spans="1:165" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:165">
       <c r="K32" s="37"/>
       <c r="L32" s="37"/>
       <c r="M32" s="37"/>
@@ -5633,7 +5709,7 @@
       <c r="FH32" s="37"/>
       <c r="FI32" s="37"/>
     </row>
-    <row r="33" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="33" spans="11:165">
       <c r="K33" s="37"/>
       <c r="L33" s="37"/>
       <c r="M33" s="37"/>
@@ -5790,7 +5866,7 @@
       <c r="FH33" s="37"/>
       <c r="FI33" s="37"/>
     </row>
-    <row r="34" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="34" spans="11:165">
       <c r="K34" s="37"/>
       <c r="L34" s="37"/>
       <c r="M34" s="37"/>
@@ -5947,7 +6023,7 @@
       <c r="FH34" s="37"/>
       <c r="FI34" s="37"/>
     </row>
-    <row r="35" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="35" spans="11:165">
       <c r="K35" s="37"/>
       <c r="L35" s="37"/>
       <c r="M35" s="37"/>
@@ -6104,7 +6180,7 @@
       <c r="FH35" s="37"/>
       <c r="FI35" s="37"/>
     </row>
-    <row r="36" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="36" spans="11:165">
       <c r="K36" s="37"/>
       <c r="L36" s="37"/>
       <c r="M36" s="37"/>
@@ -6261,7 +6337,7 @@
       <c r="FH36" s="37"/>
       <c r="FI36" s="37"/>
     </row>
-    <row r="37" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="37" spans="11:165">
       <c r="K37" s="37"/>
       <c r="L37" s="37"/>
       <c r="M37" s="37"/>
@@ -6418,7 +6494,7 @@
       <c r="FH37" s="37"/>
       <c r="FI37" s="37"/>
     </row>
-    <row r="38" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="38" spans="11:165">
       <c r="K38" s="37"/>
       <c r="L38" s="37"/>
       <c r="M38" s="37"/>
@@ -6575,7 +6651,7 @@
       <c r="FH38" s="37"/>
       <c r="FI38" s="37"/>
     </row>
-    <row r="39" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="39" spans="11:165">
       <c r="K39" s="37"/>
       <c r="L39" s="37"/>
       <c r="M39" s="37"/>
@@ -6732,7 +6808,7 @@
       <c r="FH39" s="37"/>
       <c r="FI39" s="37"/>
     </row>
-    <row r="40" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="40" spans="11:165">
       <c r="K40" s="37"/>
       <c r="L40" s="37"/>
       <c r="M40" s="37"/>
@@ -6889,7 +6965,7 @@
       <c r="FH40" s="37"/>
       <c r="FI40" s="37"/>
     </row>
-    <row r="41" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="41" spans="11:165">
       <c r="K41" s="37"/>
       <c r="L41" s="37"/>
       <c r="M41" s="37"/>
@@ -7046,7 +7122,7 @@
       <c r="FH41" s="37"/>
       <c r="FI41" s="37"/>
     </row>
-    <row r="42" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="42" spans="11:165">
       <c r="K42" s="37"/>
       <c r="L42" s="37"/>
       <c r="M42" s="37"/>
@@ -7203,7 +7279,7 @@
       <c r="FH42" s="37"/>
       <c r="FI42" s="37"/>
     </row>
-    <row r="43" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="43" spans="11:165">
       <c r="K43" s="37"/>
       <c r="L43" s="37"/>
       <c r="M43" s="37"/>
@@ -7360,7 +7436,7 @@
       <c r="FH43" s="37"/>
       <c r="FI43" s="37"/>
     </row>
-    <row r="44" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="44" spans="11:165">
       <c r="K44" s="37"/>
       <c r="L44" s="37"/>
       <c r="M44" s="37"/>
@@ -7517,7 +7593,7 @@
       <c r="FH44" s="37"/>
       <c r="FI44" s="37"/>
     </row>
-    <row r="45" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="45" spans="11:165">
       <c r="K45" s="37"/>
       <c r="L45" s="37"/>
       <c r="M45" s="37"/>
@@ -7674,7 +7750,7 @@
       <c r="FH45" s="37"/>
       <c r="FI45" s="37"/>
     </row>
-    <row r="46" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="46" spans="11:165">
       <c r="K46" s="37"/>
       <c r="L46" s="37"/>
       <c r="M46" s="37"/>
@@ -7831,7 +7907,7 @@
       <c r="FH46" s="37"/>
       <c r="FI46" s="37"/>
     </row>
-    <row r="47" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="47" spans="11:165">
       <c r="K47" s="37"/>
       <c r="L47" s="37"/>
       <c r="M47" s="37"/>
@@ -7988,7 +8064,7 @@
       <c r="FH47" s="37"/>
       <c r="FI47" s="37"/>
     </row>
-    <row r="48" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="48" spans="11:165">
       <c r="K48" s="37"/>
       <c r="L48" s="37"/>
       <c r="M48" s="37"/>
@@ -8145,7 +8221,7 @@
       <c r="FH48" s="37"/>
       <c r="FI48" s="37"/>
     </row>
-    <row r="49" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="49" spans="11:165">
       <c r="K49" s="37"/>
       <c r="L49" s="37"/>
       <c r="M49" s="37"/>
@@ -8302,7 +8378,7 @@
       <c r="FH49" s="37"/>
       <c r="FI49" s="37"/>
     </row>
-    <row r="50" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="50" spans="11:165">
       <c r="K50" s="37"/>
       <c r="L50" s="37"/>
       <c r="M50" s="37"/>
@@ -8459,7 +8535,7 @@
       <c r="FH50" s="37"/>
       <c r="FI50" s="37"/>
     </row>
-    <row r="51" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="51" spans="11:165">
       <c r="K51" s="37"/>
       <c r="L51" s="37"/>
       <c r="M51" s="37"/>
@@ -8616,7 +8692,7 @@
       <c r="FH51" s="37"/>
       <c r="FI51" s="37"/>
     </row>
-    <row r="52" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="52" spans="11:165">
       <c r="K52" s="37"/>
       <c r="L52" s="37"/>
       <c r="M52" s="37"/>
@@ -8773,7 +8849,7 @@
       <c r="FH52" s="37"/>
       <c r="FI52" s="37"/>
     </row>
-    <row r="53" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="53" spans="11:165">
       <c r="K53" s="37"/>
       <c r="L53" s="37"/>
       <c r="M53" s="37"/>
@@ -8930,7 +9006,7 @@
       <c r="FH53" s="37"/>
       <c r="FI53" s="37"/>
     </row>
-    <row r="54" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="54" spans="11:165">
       <c r="K54" s="37"/>
       <c r="L54" s="37"/>
       <c r="M54" s="37"/>
@@ -9087,7 +9163,7 @@
       <c r="FH54" s="37"/>
       <c r="FI54" s="37"/>
     </row>
-    <row r="55" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="55" spans="11:165">
       <c r="K55" s="37"/>
       <c r="L55" s="37"/>
       <c r="M55" s="37"/>
@@ -9244,7 +9320,7 @@
       <c r="FH55" s="37"/>
       <c r="FI55" s="37"/>
     </row>
-    <row r="56" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="56" spans="11:165">
       <c r="K56" s="37"/>
       <c r="L56" s="37"/>
       <c r="M56" s="37"/>
@@ -9401,7 +9477,7 @@
       <c r="FH56" s="37"/>
       <c r="FI56" s="37"/>
     </row>
-    <row r="57" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="57" spans="11:165">
       <c r="K57" s="37"/>
       <c r="L57" s="37"/>
       <c r="M57" s="37"/>
@@ -9558,7 +9634,7 @@
       <c r="FH57" s="37"/>
       <c r="FI57" s="37"/>
     </row>
-    <row r="58" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="58" spans="11:165">
       <c r="K58" s="37"/>
       <c r="L58" s="37"/>
       <c r="M58" s="37"/>
@@ -9715,7 +9791,7 @@
       <c r="FH58" s="37"/>
       <c r="FI58" s="37"/>
     </row>
-    <row r="59" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="59" spans="11:165">
       <c r="K59" s="37"/>
       <c r="L59" s="37"/>
       <c r="M59" s="37"/>
@@ -9872,7 +9948,7 @@
       <c r="FH59" s="37"/>
       <c r="FI59" s="37"/>
     </row>
-    <row r="60" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="60" spans="11:165">
       <c r="K60" s="37"/>
       <c r="L60" s="37"/>
       <c r="M60" s="37"/>
@@ -10029,7 +10105,7 @@
       <c r="FH60" s="37"/>
       <c r="FI60" s="37"/>
     </row>
-    <row r="61" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="61" spans="11:165">
       <c r="K61" s="37"/>
       <c r="L61" s="37"/>
       <c r="M61" s="37"/>
@@ -10186,7 +10262,7 @@
       <c r="FH61" s="37"/>
       <c r="FI61" s="37"/>
     </row>
-    <row r="62" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="62" spans="11:165">
       <c r="K62" s="37"/>
       <c r="L62" s="37"/>
       <c r="M62" s="37"/>
@@ -10343,7 +10419,7 @@
       <c r="FH62" s="37"/>
       <c r="FI62" s="37"/>
     </row>
-    <row r="63" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="63" spans="11:165">
       <c r="K63" s="37"/>
       <c r="L63" s="37"/>
       <c r="M63" s="37"/>
@@ -10500,7 +10576,7 @@
       <c r="FH63" s="37"/>
       <c r="FI63" s="37"/>
     </row>
-    <row r="64" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="64" spans="11:165">
       <c r="K64" s="37"/>
       <c r="L64" s="37"/>
       <c r="M64" s="37"/>
@@ -10657,7 +10733,7 @@
       <c r="FH64" s="37"/>
       <c r="FI64" s="37"/>
     </row>
-    <row r="65" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="65" spans="11:165">
       <c r="K65" s="37"/>
       <c r="L65" s="37"/>
       <c r="M65" s="37"/>
@@ -10814,7 +10890,7 @@
       <c r="FH65" s="37"/>
       <c r="FI65" s="37"/>
     </row>
-    <row r="66" spans="11:165" x14ac:dyDescent="0.4">
+    <row r="66" spans="11:165">
       <c r="K66" s="37"/>
       <c r="L66" s="37"/>
       <c r="M66" s="37"/>
@@ -10990,7 +11066,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{7ED5A534-4D62-4EE2-A79F-D52A648C4E37}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
       <formula1>"Pass, Fail, Blocked, N/A, not excuted "</formula1>
     </dataValidation>
   </dataValidations>
@@ -10999,23 +11075,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2880C1-311C-4561-94F0-88FDBC886A75}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="57" workbookViewId="0">
+      <selection activeCell="D18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.77734375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="47.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" style="8" customWidth="1"/>
     <col min="3" max="3" width="38" style="8" customWidth="1"/>
-    <col min="4" max="4" width="62.21875" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="8"/>
+    <col min="4" max="4" width="62.28515625" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -11029,7 +11105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="37.5">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -11043,7 +11119,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -11057,7 +11133,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="4" t="s">
         <v>111</v>
       </c>
@@ -11071,17 +11147,31 @@
         <v>45790</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="6">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75">
+      <c r="A6" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="6">
         <v>45790</v>
       </c>
     </row>

</xml_diff>